<commit_message>
new training modes added
</commit_message>
<xml_diff>
--- a/HSK1.xlsx
+++ b/HSK1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="37395" windowHeight="17955"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="19176" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -840,12 +841,6 @@
     <t>谁</t>
   </si>
   <si>
-    <t>shéi</t>
-  </si>
-  <si>
-    <t>who; also pronounced shui2</t>
-  </si>
-  <si>
     <t>什么</t>
   </si>
   <si>
@@ -903,9 +898,6 @@
     <t>水果</t>
   </si>
   <si>
-    <t>shuǐguǒ</t>
-  </si>
-  <si>
     <t>fruit</t>
   </si>
   <si>
@@ -1810,6 +1802,15 @@
   </si>
   <si>
     <t>https://www.hsk.academy/static/audio/mp3/words/昨天.mp3</t>
+  </si>
+  <si>
+    <t>shuǐ guǒ</t>
+  </si>
+  <si>
+    <t>shuí</t>
+  </si>
+  <si>
+    <t>who</t>
   </si>
 </sst>
 </file>
@@ -1859,10 +1860,10 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2167,20 +2168,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="B34" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="14.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="62.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="68.7109375" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="2" max="2" width="14.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="68.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="62.33203125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2188,13 +2189,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>448</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -2202,13 +2203,13 @@
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>449</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -2216,14 +2217,14 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>533</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q3" s="3"/>
-    </row>
-    <row r="4" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>530</v>
+      </c>
+      <c r="Q3" s="2"/>
+    </row>
+    <row r="4" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -2231,13 +2232,13 @@
         <v>13</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>534</v>
+        <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -2245,13 +2246,13 @@
         <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>532</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -2259,13 +2260,13 @@
         <v>16</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>450</v>
+        <v>17</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -2273,13 +2274,13 @@
         <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>451</v>
+        <v>23</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -2287,13 +2288,13 @@
         <v>19</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>535</v>
+        <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -2301,13 +2302,13 @@
         <v>25</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>452</v>
+        <v>26</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -2315,13 +2316,13 @@
         <v>28</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>453</v>
+        <v>29</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -2329,13 +2330,13 @@
         <v>31</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>454</v>
+        <v>32</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
@@ -2343,13 +2344,13 @@
         <v>34</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>536</v>
+        <v>35</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>39</v>
       </c>
@@ -2357,13 +2358,13 @@
         <v>40</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>455</v>
+        <v>41</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
@@ -2371,13 +2372,13 @@
         <v>37</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>537</v>
+        <v>38</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>42</v>
       </c>
@@ -2385,13 +2386,13 @@
         <v>43</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>456</v>
+        <v>44</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>45</v>
       </c>
@@ -2399,13 +2400,13 @@
         <v>46</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>457</v>
+        <v>47</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>48</v>
       </c>
@@ -2413,13 +2414,13 @@
         <v>49</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>538</v>
+        <v>50</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>51</v>
       </c>
@@ -2427,13 +2428,13 @@
         <v>52</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>539</v>
+        <v>53</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>54</v>
       </c>
@@ -2441,13 +2442,13 @@
         <v>55</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>540</v>
+        <v>56</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>57</v>
       </c>
@@ -2455,13 +2456,13 @@
         <v>58</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>541</v>
+        <v>59</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>60</v>
       </c>
@@ -2469,13 +2470,13 @@
         <v>61</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>458</v>
+        <v>62</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>63</v>
       </c>
@@ -2483,13 +2484,13 @@
         <v>64</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>459</v>
+        <v>65</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>66</v>
       </c>
@@ -2497,13 +2498,13 @@
         <v>67</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>542</v>
+        <v>68</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>69</v>
       </c>
@@ -2511,13 +2512,13 @@
         <v>70</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>460</v>
+        <v>71</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>72</v>
       </c>
@@ -2525,13 +2526,13 @@
         <v>73</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>543</v>
+        <v>74</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>78</v>
       </c>
@@ -2539,13 +2540,13 @@
         <v>79</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>461</v>
+        <v>80</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>75</v>
       </c>
@@ -2553,13 +2554,13 @@
         <v>76</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>544</v>
+        <v>77</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>81</v>
       </c>
@@ -2567,13 +2568,13 @@
         <v>82</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>545</v>
+        <v>83</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>84</v>
       </c>
@@ -2581,13 +2582,13 @@
         <v>85</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>546</v>
+        <v>86</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>87</v>
       </c>
@@ -2595,13 +2596,13 @@
         <v>88</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>547</v>
+        <v>89</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>90</v>
       </c>
@@ -2609,13 +2610,13 @@
         <v>91</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>548</v>
+        <v>92</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>93</v>
       </c>
@@ -2623,13 +2624,13 @@
         <v>94</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>462</v>
+        <v>95</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>96</v>
       </c>
@@ -2637,13 +2638,13 @@
         <v>97</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>549</v>
+        <v>98</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>99</v>
       </c>
@@ -2651,13 +2652,13 @@
         <v>100</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>463</v>
+        <v>101</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>102</v>
       </c>
@@ -2665,13 +2666,13 @@
         <v>103</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>550</v>
+        <v>104</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>108</v>
       </c>
@@ -2679,13 +2680,13 @@
         <v>109</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>464</v>
+        <v>110</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>105</v>
       </c>
@@ -2693,13 +2694,13 @@
         <v>106</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>465</v>
+        <v>107</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>114</v>
       </c>
@@ -2707,13 +2708,13 @@
         <v>115</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>466</v>
+        <v>116</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>111</v>
       </c>
@@ -2721,13 +2722,13 @@
         <v>112</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>467</v>
+        <v>113</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>117</v>
       </c>
@@ -2735,13 +2736,13 @@
         <v>118</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>468</v>
+        <v>119</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>120</v>
       </c>
@@ -2749,13 +2750,13 @@
         <v>121</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>551</v>
+        <v>122</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>123</v>
       </c>
@@ -2763,13 +2764,13 @@
         <v>124</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>469</v>
+        <v>125</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>126</v>
       </c>
@@ -2777,13 +2778,13 @@
         <v>127</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>470</v>
+        <v>128</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>129</v>
       </c>
@@ -2791,13 +2792,13 @@
         <v>130</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>471</v>
+        <v>131</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>132</v>
       </c>
@@ -2805,13 +2806,13 @@
         <v>133</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>472</v>
+        <v>134</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>135</v>
       </c>
@@ -2819,13 +2820,13 @@
         <v>136</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>473</v>
+        <v>137</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>138</v>
       </c>
@@ -2833,13 +2834,13 @@
         <v>139</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>552</v>
+        <v>140</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>141</v>
       </c>
@@ -2847,13 +2848,13 @@
         <v>142</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>474</v>
+        <v>143</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>144</v>
       </c>
@@ -2861,13 +2862,13 @@
         <v>145</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>475</v>
+        <v>146</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>147</v>
       </c>
@@ -2875,13 +2876,13 @@
         <v>148</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>476</v>
+        <v>149</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>150</v>
       </c>
@@ -2889,13 +2890,13 @@
         <v>151</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>553</v>
+        <v>152</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>153</v>
       </c>
@@ -2903,13 +2904,13 @@
         <v>154</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>477</v>
+        <v>155</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>156</v>
       </c>
@@ -2917,13 +2918,13 @@
         <v>157</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>478</v>
+        <v>158</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>159</v>
       </c>
@@ -2931,13 +2932,13 @@
         <v>160</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>554</v>
+        <v>161</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>162</v>
       </c>
@@ -2945,13 +2946,13 @@
         <v>163</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>479</v>
+        <v>164</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>165</v>
       </c>
@@ -2959,13 +2960,13 @@
         <v>166</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>480</v>
+        <v>167</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>168</v>
       </c>
@@ -2973,13 +2974,13 @@
         <v>169</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>481</v>
+        <v>170</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>171</v>
       </c>
@@ -2987,13 +2988,13 @@
         <v>172</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>482</v>
+        <v>173</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>174</v>
       </c>
@@ -3001,13 +3002,13 @@
         <v>175</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>483</v>
+        <v>176</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>177</v>
       </c>
@@ -3015,13 +3016,13 @@
         <v>178</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>555</v>
+        <v>179</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>180</v>
       </c>
@@ -3029,13 +3030,13 @@
         <v>181</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>484</v>
+        <v>182</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>183</v>
       </c>
@@ -3043,13 +3044,13 @@
         <v>184</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>485</v>
+        <v>185</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>186</v>
       </c>
@@ -3057,13 +3058,13 @@
         <v>187</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>556</v>
+        <v>188</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>189</v>
       </c>
@@ -3071,13 +3072,13 @@
         <v>190</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>557</v>
+        <v>191</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>192</v>
       </c>
@@ -3085,13 +3086,13 @@
         <v>193</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>558</v>
+        <v>194</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>198</v>
       </c>
@@ -3099,13 +3100,13 @@
         <v>199</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>559</v>
+        <v>200</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>195</v>
       </c>
@@ -3113,13 +3114,13 @@
         <v>196</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>560</v>
+        <v>197</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>207</v>
       </c>
@@ -3127,13 +3128,13 @@
         <v>208</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>486</v>
+        <v>209</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>201</v>
       </c>
@@ -3141,13 +3142,13 @@
         <v>202</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>487</v>
+        <v>203</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>204</v>
       </c>
@@ -3155,13 +3156,13 @@
         <v>205</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>561</v>
+        <v>206</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>210</v>
       </c>
@@ -3169,13 +3170,13 @@
         <v>211</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>488</v>
+        <v>212</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>213</v>
       </c>
@@ -3183,13 +3184,13 @@
         <v>214</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>489</v>
+        <v>215</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>216</v>
       </c>
@@ -3197,13 +3198,13 @@
         <v>217</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>490</v>
+        <v>218</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>219</v>
       </c>
@@ -3211,13 +3212,13 @@
         <v>220</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>491</v>
+        <v>221</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>222</v>
       </c>
@@ -3225,13 +3226,13 @@
         <v>223</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>492</v>
+        <v>224</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>225</v>
       </c>
@@ -3239,13 +3240,13 @@
         <v>226</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>562</v>
+        <v>227</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>228</v>
       </c>
@@ -3253,13 +3254,13 @@
         <v>229</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>563</v>
+        <v>230</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>231</v>
       </c>
@@ -3267,13 +3268,13 @@
         <v>232</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>564</v>
+        <v>233</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>234</v>
       </c>
@@ -3281,13 +3282,13 @@
         <v>235</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>493</v>
+        <v>236</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>240</v>
       </c>
@@ -3295,13 +3296,13 @@
         <v>241</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>494</v>
+        <v>242</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>237</v>
       </c>
@@ -3309,13 +3310,13 @@
         <v>238</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>565</v>
+        <v>239</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>243</v>
       </c>
@@ -3323,13 +3324,13 @@
         <v>244</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>495</v>
+        <v>245</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>246</v>
       </c>
@@ -3337,13 +3338,13 @@
         <v>247</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>496</v>
+        <v>248</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>249</v>
       </c>
@@ -3351,13 +3352,13 @@
         <v>250</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>497</v>
+        <v>251</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>252</v>
       </c>
@@ -3365,13 +3366,13 @@
         <v>253</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>498</v>
+        <v>254</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>255</v>
       </c>
@@ -3379,13 +3380,13 @@
         <v>256</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>566</v>
+        <v>257</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>258</v>
       </c>
@@ -3393,13 +3394,13 @@
         <v>259</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>499</v>
+        <v>260</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>264</v>
       </c>
@@ -3407,13 +3408,13 @@
         <v>265</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>500</v>
+        <v>266</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>261</v>
       </c>
@@ -3421,13 +3422,13 @@
         <v>262</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>567</v>
+        <v>263</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>267</v>
       </c>
@@ -3435,13 +3436,13 @@
         <v>268</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>568</v>
+        <v>269</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>270</v>
       </c>
@@ -3449,836 +3450,836 @@
         <v>271</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>501</v>
+        <v>272</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>273</v>
       </c>
       <c r="B92" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>597</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="C92" s="3" t="s">
+      <c r="B93" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="D97" s="2" t="s">
         <v>502</v>
       </c>
-      <c r="D92" s="2" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="C93" s="3" t="s">
+    </row>
+    <row r="98" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="D100" s="2" t="s">
         <v>569</v>
       </c>
-      <c r="D93" s="2" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="C94" s="3" t="s">
-        <v>503</v>
-      </c>
-      <c r="D94" s="2" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="C95" s="3" t="s">
+    </row>
+    <row r="101" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="D101" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="D95" s="2" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="C96" s="3" t="s">
+    </row>
+    <row r="102" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="D107" s="2" t="s">
         <v>570</v>
       </c>
-      <c r="D96" s="2" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="C97" s="3" t="s">
-        <v>505</v>
-      </c>
-      <c r="D97" s="2" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="C98" s="3" t="s">
-        <v>506</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="C99" s="3" t="s">
+    </row>
+    <row r="108" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="D109" s="2" t="s">
         <v>571</v>
       </c>
-      <c r="D99" s="2" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="C100" s="3" t="s">
+    </row>
+    <row r="110" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="D112" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="D100" s="2" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="C101" s="3" t="s">
-        <v>507</v>
-      </c>
-      <c r="D101" s="2" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="C102" s="3" t="s">
-        <v>508</v>
-      </c>
-      <c r="D102" s="2" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="C103" s="3" t="s">
-        <v>509</v>
-      </c>
-      <c r="D103" s="2" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="C104" s="3" t="s">
-        <v>510</v>
-      </c>
-      <c r="D104" s="2" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="C105" s="3" t="s">
-        <v>511</v>
-      </c>
-      <c r="D105" s="2" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="B106" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="C106" s="3" t="s">
-        <v>512</v>
-      </c>
-      <c r="D106" s="2" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="C107" s="3" t="s">
+    </row>
+    <row r="113" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="D114" s="2" t="s">
         <v>573</v>
       </c>
-      <c r="D107" s="2" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="C108" s="3" t="s">
-        <v>513</v>
-      </c>
-      <c r="D108" s="2" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="C109" s="3" t="s">
+    </row>
+    <row r="115" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="D116" s="2" t="s">
         <v>574</v>
       </c>
-      <c r="D109" s="2" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="C110" s="3" t="s">
-        <v>514</v>
-      </c>
-      <c r="D110" s="2" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="C111" s="3" t="s">
+    </row>
+    <row r="117" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="D120" s="2" t="s">
         <v>515</v>
       </c>
-      <c r="D111" s="2" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C112" s="3" t="s">
-        <v>575</v>
-      </c>
-      <c r="D112" s="2" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="C113" s="3" t="s">
+    </row>
+    <row r="121" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="D121" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="D113" s="2" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="C114" s="3" t="s">
-        <v>576</v>
-      </c>
-      <c r="D114" s="2" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="C115" s="3" t="s">
+    </row>
+    <row r="122" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A123" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="D123" s="2" t="s">
         <v>517</v>
       </c>
-      <c r="D115" s="2" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="C116" s="3" t="s">
-        <v>577</v>
-      </c>
-      <c r="D116" s="2" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="C117" s="3" t="s">
-        <v>578</v>
-      </c>
-      <c r="D117" s="2" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C118" s="3" t="s">
+    </row>
+    <row r="124" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="D125" s="2" t="s">
         <v>579</v>
       </c>
-      <c r="D118" s="2" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="C119" s="3" t="s">
+    </row>
+    <row r="126" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A126" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="D126" s="2" t="s">
         <v>580</v>
       </c>
-      <c r="D119" s="2" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="B120" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="C120" s="3" t="s">
-        <v>518</v>
-      </c>
-      <c r="D120" s="2" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="B121" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="C121" s="3" t="s">
+    </row>
+    <row r="127" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="D127" s="2" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="D128" s="2" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="D129" s="2" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="D130" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="D121" s="2" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="B122" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="C122" s="3" t="s">
-        <v>581</v>
-      </c>
-      <c r="D122" s="2" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="B123" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="C123" s="3" t="s">
+    </row>
+    <row r="131" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A131" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A132" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="D132" s="2" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="D133" s="2" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A134" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="D134" s="2" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A135" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="D135" s="2" t="s">
         <v>520</v>
       </c>
-      <c r="D123" s="2" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="B124" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="C124" s="3" t="s">
+    </row>
+    <row r="136" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A136" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="D136" s="2" t="s">
         <v>521</v>
       </c>
-      <c r="D124" s="2" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="B125" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="C125" s="3" t="s">
-        <v>582</v>
-      </c>
-      <c r="D125" s="2" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="B126" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="C126" s="3" t="s">
-        <v>583</v>
-      </c>
-      <c r="D126" s="2" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="B127" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="C127" s="3" t="s">
-        <v>584</v>
-      </c>
-      <c r="D127" s="2" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="B128" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="C128" s="3" t="s">
-        <v>585</v>
-      </c>
-      <c r="D128" s="2" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="B129" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="C129" s="3" t="s">
-        <v>586</v>
-      </c>
-      <c r="D129" s="2" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="B130" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="C130" s="3" t="s">
+    </row>
+    <row r="137" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A137" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="D137" s="2" t="s">
         <v>522</v>
       </c>
-      <c r="D130" s="2" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="B131" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="C131" s="3" t="s">
-        <v>587</v>
-      </c>
-      <c r="D131" s="2" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="B132" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="C132" s="3" t="s">
+    </row>
+    <row r="138" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A138" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="C138" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="D138" s="2" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A139" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="C139" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="D139" s="2" t="s">
         <v>588</v>
       </c>
-      <c r="D132" s="2" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="B133" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="C133" s="3" t="s">
+    </row>
+    <row r="140" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A140" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="C140" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="D140" s="2" t="s">
         <v>589</v>
       </c>
-      <c r="D133" s="2" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="B134" s="1" t="s">
-        <v>396</v>
-      </c>
-      <c r="C134" s="3" t="s">
+    </row>
+    <row r="141" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A141" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="C141" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="D141" s="2" t="s">
         <v>590</v>
       </c>
-      <c r="D134" s="2" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="B135" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="C135" s="3" t="s">
-        <v>523</v>
-      </c>
-      <c r="D135" s="2" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="B136" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="C136" s="3" t="s">
+    </row>
+    <row r="142" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A142" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="C142" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="D142" s="2" t="s">
         <v>524</v>
       </c>
-      <c r="D136" s="2" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="B137" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="C137" s="3" t="s">
+    </row>
+    <row r="143" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A143" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="C143" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="D143" s="2" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A144" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="C144" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="D144" s="2" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A145" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="C145" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="D145" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="D137" s="2" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="B138" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="C138" s="3" t="s">
+    </row>
+    <row r="146" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A146" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="D146" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A147" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="C147" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="D147" s="2" t="s">
         <v>526</v>
       </c>
-      <c r="D138" s="2" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="B139" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="C139" s="3" t="s">
-        <v>591</v>
-      </c>
-      <c r="D139" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="B140" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="C140" s="3" t="s">
-        <v>592</v>
-      </c>
-      <c r="D140" s="2" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="B141" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="C141" s="3" t="s">
-        <v>593</v>
-      </c>
-      <c r="D141" s="2" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="B142" s="1" t="s">
-        <v>423</v>
-      </c>
-      <c r="C142" s="3" t="s">
+    </row>
+    <row r="148" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A148" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="C148" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="D148" s="2" t="s">
         <v>527</v>
       </c>
-      <c r="D142" s="2" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="B143" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="C143" s="3" t="s">
+    </row>
+    <row r="149" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A149" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="C149" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="D149" s="2" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A150" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="C150" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="D150" s="2" t="s">
         <v>594</v>
-      </c>
-      <c r="D143" s="2" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="1" t="s">
-        <v>428</v>
-      </c>
-      <c r="B144" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="C144" s="3" t="s">
-        <v>595</v>
-      </c>
-      <c r="D144" s="2" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="B145" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="C145" s="3" t="s">
-        <v>528</v>
-      </c>
-      <c r="D145" s="2" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="B146" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="C146" s="3" t="s">
-        <v>596</v>
-      </c>
-      <c r="D146" s="2" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="B147" s="1" t="s">
-        <v>438</v>
-      </c>
-      <c r="C147" s="3" t="s">
-        <v>529</v>
-      </c>
-      <c r="D147" s="2" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="1" t="s">
-        <v>446</v>
-      </c>
-      <c r="B148" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="C148" s="3" t="s">
-        <v>530</v>
-      </c>
-      <c r="D148" s="2" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="B149" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="C149" s="3" t="s">
-        <v>531</v>
-      </c>
-      <c r="D149" s="2" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="B150" s="1" t="s">
-        <v>441</v>
-      </c>
-      <c r="C150" s="3" t="s">
-        <v>597</v>
-      </c>
-      <c r="D150" s="2" t="s">
-        <v>442</v>
       </c>
     </row>
   </sheetData>
@@ -4286,156 +4287,156 @@
     <sortCondition ref="B1:B150"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="C1" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C12" r:id="rId3"/>
-    <hyperlink ref="C14" r:id="rId4"/>
-    <hyperlink ref="C17" r:id="rId5"/>
-    <hyperlink ref="C80" r:id="rId6"/>
-    <hyperlink ref="C57" r:id="rId7"/>
-    <hyperlink ref="C21" r:id="rId8"/>
-    <hyperlink ref="C68" r:id="rId9"/>
-    <hyperlink ref="C142" r:id="rId10"/>
-    <hyperlink ref="C92" r:id="rId11"/>
-    <hyperlink ref="C22" r:id="rId12"/>
-    <hyperlink ref="C82" r:id="rId13"/>
-    <hyperlink ref="C101" r:id="rId14"/>
-    <hyperlink ref="C10" r:id="rId15"/>
-    <hyperlink ref="C72" r:id="rId16"/>
-    <hyperlink ref="C50" r:id="rId17"/>
-    <hyperlink ref="C15" r:id="rId18"/>
-    <hyperlink ref="C62" r:id="rId19"/>
-    <hyperlink ref="C34" r:id="rId20"/>
-    <hyperlink ref="C84" r:id="rId21"/>
-    <hyperlink ref="C98" r:id="rId22"/>
-    <hyperlink ref="C135" r:id="rId23"/>
-    <hyperlink ref="C6" r:id="rId24"/>
-    <hyperlink ref="C136" r:id="rId25"/>
-    <hyperlink ref="C137" r:id="rId26"/>
-    <hyperlink ref="C111" r:id="rId27"/>
-    <hyperlink ref="C120" r:id="rId28"/>
-    <hyperlink ref="C40" r:id="rId29"/>
-    <hyperlink ref="C74" r:id="rId30"/>
-    <hyperlink ref="C103" r:id="rId31"/>
-    <hyperlink ref="C91" r:id="rId32"/>
-    <hyperlink ref="C121" r:id="rId33"/>
-    <hyperlink ref="C147" r:id="rId34"/>
-    <hyperlink ref="C37" r:id="rId35"/>
-    <hyperlink ref="C104" r:id="rId36"/>
-    <hyperlink ref="C106" r:id="rId37"/>
-    <hyperlink ref="C13" r:id="rId38"/>
-    <hyperlink ref="C24" r:id="rId39"/>
-    <hyperlink ref="C52" r:id="rId40"/>
-    <hyperlink ref="C138" r:id="rId41"/>
-    <hyperlink ref="C102" r:id="rId42"/>
-    <hyperlink ref="C39" r:id="rId43"/>
-    <hyperlink ref="C110" r:id="rId44"/>
-    <hyperlink ref="C69" r:id="rId45"/>
-    <hyperlink ref="C71" r:id="rId46"/>
-    <hyperlink ref="C108" r:id="rId47"/>
-    <hyperlink ref="C59" r:id="rId48"/>
-    <hyperlink ref="C11" r:id="rId49"/>
-    <hyperlink ref="C36" r:id="rId50"/>
-    <hyperlink ref="C46" r:id="rId51"/>
-    <hyperlink ref="C83" r:id="rId52"/>
-    <hyperlink ref="C94" r:id="rId53"/>
-    <hyperlink ref="C44" r:id="rId54"/>
-    <hyperlink ref="C56" r:id="rId55"/>
-    <hyperlink ref="C123" r:id="rId56"/>
-    <hyperlink ref="C58" r:id="rId57"/>
-    <hyperlink ref="C2" r:id="rId58"/>
-    <hyperlink ref="C149" r:id="rId59"/>
-    <hyperlink ref="C73" r:id="rId60"/>
-    <hyperlink ref="C145" r:id="rId61"/>
-    <hyperlink ref="C43" r:id="rId62"/>
-    <hyperlink ref="C105" r:id="rId63"/>
-    <hyperlink ref="C85" r:id="rId64"/>
-    <hyperlink ref="C124" r:id="rId65"/>
-    <hyperlink ref="C113" r:id="rId66"/>
-    <hyperlink ref="C26" r:id="rId67"/>
-    <hyperlink ref="C55" r:id="rId68"/>
-    <hyperlink ref="C61" r:id="rId69"/>
-    <hyperlink ref="C97" r:id="rId70"/>
-    <hyperlink ref="C48" r:id="rId71"/>
-    <hyperlink ref="C32" r:id="rId72"/>
-    <hyperlink ref="C7" r:id="rId73"/>
-    <hyperlink ref="C115" r:id="rId74"/>
-    <hyperlink ref="C88" r:id="rId75"/>
-    <hyperlink ref="C87" r:id="rId76"/>
-    <hyperlink ref="C79" r:id="rId77"/>
-    <hyperlink ref="C130" r:id="rId78"/>
-    <hyperlink ref="C4" r:id="rId79"/>
-    <hyperlink ref="C5" r:id="rId80"/>
-    <hyperlink ref="C8" r:id="rId81"/>
-    <hyperlink ref="C18" r:id="rId82"/>
-    <hyperlink ref="C19" r:id="rId83"/>
-    <hyperlink ref="C20" r:id="rId84"/>
-    <hyperlink ref="C23" r:id="rId85"/>
-    <hyperlink ref="C25" r:id="rId86"/>
-    <hyperlink ref="C27" r:id="rId87"/>
-    <hyperlink ref="C28" r:id="rId88"/>
-    <hyperlink ref="C29" r:id="rId89"/>
-    <hyperlink ref="C30" r:id="rId90"/>
-    <hyperlink ref="C31" r:id="rId91"/>
-    <hyperlink ref="C33" r:id="rId92"/>
-    <hyperlink ref="C35" r:id="rId93"/>
-    <hyperlink ref="C41" r:id="rId94"/>
-    <hyperlink ref="C47" r:id="rId95"/>
-    <hyperlink ref="C51" r:id="rId96"/>
-    <hyperlink ref="C54" r:id="rId97"/>
-    <hyperlink ref="C60" r:id="rId98"/>
-    <hyperlink ref="C63" r:id="rId99"/>
-    <hyperlink ref="C64" r:id="rId100"/>
-    <hyperlink ref="C65" r:id="rId101"/>
-    <hyperlink ref="C66" r:id="rId102"/>
-    <hyperlink ref="C67" r:id="rId103"/>
-    <hyperlink ref="C70" r:id="rId104"/>
-    <hyperlink ref="C76" r:id="rId105"/>
-    <hyperlink ref="C77" r:id="rId106"/>
-    <hyperlink ref="C78" r:id="rId107"/>
-    <hyperlink ref="C81" r:id="rId108"/>
-    <hyperlink ref="C86" r:id="rId109"/>
-    <hyperlink ref="C89" r:id="rId110"/>
-    <hyperlink ref="C90" r:id="rId111"/>
-    <hyperlink ref="C93" r:id="rId112"/>
-    <hyperlink ref="C96" r:id="rId113"/>
-    <hyperlink ref="C99" r:id="rId114"/>
-    <hyperlink ref="C100" r:id="rId115"/>
-    <hyperlink ref="C107" r:id="rId116"/>
-    <hyperlink ref="C109" r:id="rId117"/>
-    <hyperlink ref="C112" r:id="rId118"/>
-    <hyperlink ref="C114" r:id="rId119"/>
-    <hyperlink ref="C116" r:id="rId120"/>
-    <hyperlink ref="C117" r:id="rId121"/>
-    <hyperlink ref="C118" r:id="rId122"/>
-    <hyperlink ref="C119" r:id="rId123"/>
-    <hyperlink ref="C122" r:id="rId124"/>
-    <hyperlink ref="C125" r:id="rId125"/>
-    <hyperlink ref="C126" r:id="rId126"/>
-    <hyperlink ref="C127" r:id="rId127"/>
-    <hyperlink ref="C128" r:id="rId128"/>
-    <hyperlink ref="C129" r:id="rId129"/>
-    <hyperlink ref="C131" r:id="rId130"/>
-    <hyperlink ref="C132" r:id="rId131"/>
-    <hyperlink ref="C133" r:id="rId132"/>
-    <hyperlink ref="C134" r:id="rId133"/>
-    <hyperlink ref="C139" r:id="rId134"/>
-    <hyperlink ref="C140" r:id="rId135"/>
-    <hyperlink ref="C141" r:id="rId136"/>
-    <hyperlink ref="C143" r:id="rId137"/>
-    <hyperlink ref="C144" r:id="rId138"/>
-    <hyperlink ref="C146" r:id="rId139"/>
-    <hyperlink ref="C150" r:id="rId140"/>
-    <hyperlink ref="C9" r:id="rId141"/>
-    <hyperlink ref="C16" r:id="rId142"/>
-    <hyperlink ref="C53" r:id="rId143"/>
-    <hyperlink ref="C95" r:id="rId144"/>
-    <hyperlink ref="C49" r:id="rId145"/>
-    <hyperlink ref="C45" r:id="rId146"/>
-    <hyperlink ref="C75" r:id="rId147"/>
-    <hyperlink ref="C42" r:id="rId148"/>
-    <hyperlink ref="C148" r:id="rId149"/>
-    <hyperlink ref="C38" r:id="rId150"/>
+    <hyperlink ref="D1" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D12" r:id="rId3"/>
+    <hyperlink ref="D14" r:id="rId4"/>
+    <hyperlink ref="D17" r:id="rId5"/>
+    <hyperlink ref="D80" r:id="rId6"/>
+    <hyperlink ref="D57" r:id="rId7"/>
+    <hyperlink ref="D21" r:id="rId8"/>
+    <hyperlink ref="D68" r:id="rId9"/>
+    <hyperlink ref="D142" r:id="rId10"/>
+    <hyperlink ref="D92" r:id="rId11"/>
+    <hyperlink ref="D22" r:id="rId12"/>
+    <hyperlink ref="D82" r:id="rId13"/>
+    <hyperlink ref="D101" r:id="rId14"/>
+    <hyperlink ref="D10" r:id="rId15"/>
+    <hyperlink ref="D72" r:id="rId16"/>
+    <hyperlink ref="D50" r:id="rId17"/>
+    <hyperlink ref="D15" r:id="rId18"/>
+    <hyperlink ref="D62" r:id="rId19"/>
+    <hyperlink ref="D34" r:id="rId20"/>
+    <hyperlink ref="D84" r:id="rId21"/>
+    <hyperlink ref="D98" r:id="rId22"/>
+    <hyperlink ref="D135" r:id="rId23"/>
+    <hyperlink ref="D6" r:id="rId24"/>
+    <hyperlink ref="D136" r:id="rId25"/>
+    <hyperlink ref="D137" r:id="rId26"/>
+    <hyperlink ref="D111" r:id="rId27"/>
+    <hyperlink ref="D120" r:id="rId28"/>
+    <hyperlink ref="D40" r:id="rId29"/>
+    <hyperlink ref="D74" r:id="rId30"/>
+    <hyperlink ref="D103" r:id="rId31"/>
+    <hyperlink ref="D91" r:id="rId32"/>
+    <hyperlink ref="D121" r:id="rId33"/>
+    <hyperlink ref="D147" r:id="rId34"/>
+    <hyperlink ref="D37" r:id="rId35"/>
+    <hyperlink ref="D104" r:id="rId36"/>
+    <hyperlink ref="D106" r:id="rId37"/>
+    <hyperlink ref="D13" r:id="rId38"/>
+    <hyperlink ref="D24" r:id="rId39"/>
+    <hyperlink ref="D52" r:id="rId40"/>
+    <hyperlink ref="D138" r:id="rId41"/>
+    <hyperlink ref="D102" r:id="rId42"/>
+    <hyperlink ref="D39" r:id="rId43"/>
+    <hyperlink ref="D110" r:id="rId44"/>
+    <hyperlink ref="D69" r:id="rId45"/>
+    <hyperlink ref="D71" r:id="rId46"/>
+    <hyperlink ref="D108" r:id="rId47"/>
+    <hyperlink ref="D59" r:id="rId48"/>
+    <hyperlink ref="D11" r:id="rId49"/>
+    <hyperlink ref="D36" r:id="rId50"/>
+    <hyperlink ref="D46" r:id="rId51"/>
+    <hyperlink ref="D83" r:id="rId52"/>
+    <hyperlink ref="D94" r:id="rId53"/>
+    <hyperlink ref="D44" r:id="rId54"/>
+    <hyperlink ref="D56" r:id="rId55"/>
+    <hyperlink ref="D123" r:id="rId56"/>
+    <hyperlink ref="D58" r:id="rId57"/>
+    <hyperlink ref="D2" r:id="rId58"/>
+    <hyperlink ref="D149" r:id="rId59"/>
+    <hyperlink ref="D73" r:id="rId60"/>
+    <hyperlink ref="D145" r:id="rId61"/>
+    <hyperlink ref="D43" r:id="rId62"/>
+    <hyperlink ref="D105" r:id="rId63"/>
+    <hyperlink ref="D85" r:id="rId64"/>
+    <hyperlink ref="D124" r:id="rId65"/>
+    <hyperlink ref="D113" r:id="rId66"/>
+    <hyperlink ref="D26" r:id="rId67"/>
+    <hyperlink ref="D55" r:id="rId68"/>
+    <hyperlink ref="D61" r:id="rId69"/>
+    <hyperlink ref="D97" r:id="rId70"/>
+    <hyperlink ref="D48" r:id="rId71"/>
+    <hyperlink ref="D32" r:id="rId72"/>
+    <hyperlink ref="D7" r:id="rId73"/>
+    <hyperlink ref="D115" r:id="rId74"/>
+    <hyperlink ref="D88" r:id="rId75"/>
+    <hyperlink ref="D87" r:id="rId76"/>
+    <hyperlink ref="D79" r:id="rId77"/>
+    <hyperlink ref="D130" r:id="rId78"/>
+    <hyperlink ref="D4" r:id="rId79"/>
+    <hyperlink ref="D5" r:id="rId80"/>
+    <hyperlink ref="D8" r:id="rId81"/>
+    <hyperlink ref="D18" r:id="rId82"/>
+    <hyperlink ref="D19" r:id="rId83"/>
+    <hyperlink ref="D20" r:id="rId84"/>
+    <hyperlink ref="D23" r:id="rId85"/>
+    <hyperlink ref="D25" r:id="rId86"/>
+    <hyperlink ref="D27" r:id="rId87"/>
+    <hyperlink ref="D28" r:id="rId88"/>
+    <hyperlink ref="D29" r:id="rId89"/>
+    <hyperlink ref="D30" r:id="rId90"/>
+    <hyperlink ref="D31" r:id="rId91"/>
+    <hyperlink ref="D33" r:id="rId92"/>
+    <hyperlink ref="D35" r:id="rId93"/>
+    <hyperlink ref="D41" r:id="rId94"/>
+    <hyperlink ref="D47" r:id="rId95"/>
+    <hyperlink ref="D51" r:id="rId96"/>
+    <hyperlink ref="D54" r:id="rId97"/>
+    <hyperlink ref="D60" r:id="rId98"/>
+    <hyperlink ref="D63" r:id="rId99"/>
+    <hyperlink ref="D64" r:id="rId100"/>
+    <hyperlink ref="D65" r:id="rId101"/>
+    <hyperlink ref="D66" r:id="rId102"/>
+    <hyperlink ref="D67" r:id="rId103"/>
+    <hyperlink ref="D70" r:id="rId104"/>
+    <hyperlink ref="D76" r:id="rId105"/>
+    <hyperlink ref="D77" r:id="rId106"/>
+    <hyperlink ref="D78" r:id="rId107"/>
+    <hyperlink ref="D81" r:id="rId108"/>
+    <hyperlink ref="D86" r:id="rId109"/>
+    <hyperlink ref="D89" r:id="rId110"/>
+    <hyperlink ref="D90" r:id="rId111"/>
+    <hyperlink ref="D93" r:id="rId112"/>
+    <hyperlink ref="D96" r:id="rId113"/>
+    <hyperlink ref="D99" r:id="rId114"/>
+    <hyperlink ref="D100" r:id="rId115"/>
+    <hyperlink ref="D107" r:id="rId116"/>
+    <hyperlink ref="D109" r:id="rId117"/>
+    <hyperlink ref="D112" r:id="rId118"/>
+    <hyperlink ref="D114" r:id="rId119"/>
+    <hyperlink ref="D116" r:id="rId120"/>
+    <hyperlink ref="D117" r:id="rId121"/>
+    <hyperlink ref="D118" r:id="rId122"/>
+    <hyperlink ref="D119" r:id="rId123"/>
+    <hyperlink ref="D122" r:id="rId124"/>
+    <hyperlink ref="D125" r:id="rId125"/>
+    <hyperlink ref="D126" r:id="rId126"/>
+    <hyperlink ref="D127" r:id="rId127"/>
+    <hyperlink ref="D128" r:id="rId128"/>
+    <hyperlink ref="D129" r:id="rId129"/>
+    <hyperlink ref="D131" r:id="rId130"/>
+    <hyperlink ref="D132" r:id="rId131"/>
+    <hyperlink ref="D133" r:id="rId132"/>
+    <hyperlink ref="D134" r:id="rId133"/>
+    <hyperlink ref="D139" r:id="rId134"/>
+    <hyperlink ref="D140" r:id="rId135"/>
+    <hyperlink ref="D141" r:id="rId136"/>
+    <hyperlink ref="D143" r:id="rId137"/>
+    <hyperlink ref="D144" r:id="rId138"/>
+    <hyperlink ref="D146" r:id="rId139"/>
+    <hyperlink ref="D150" r:id="rId140"/>
+    <hyperlink ref="D9" r:id="rId141"/>
+    <hyperlink ref="D16" r:id="rId142"/>
+    <hyperlink ref="D53" r:id="rId143"/>
+    <hyperlink ref="D95" r:id="rId144"/>
+    <hyperlink ref="D49" r:id="rId145"/>
+    <hyperlink ref="D45" r:id="rId146"/>
+    <hyperlink ref="D75" r:id="rId147"/>
+    <hyperlink ref="D42" r:id="rId148"/>
+    <hyperlink ref="D148" r:id="rId149"/>
+    <hyperlink ref="D38" r:id="rId150"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4447,7 +4448,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4459,7 +4460,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>